<commit_message>
ajouts binding  + example care plan 9a7e74c6ff63a487b613993ee94e019015a79f79
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/StructureDefinition-oncofair-element-form.xlsx
+++ b/update-mapping-pn13/ig/StructureDefinition-oncofair-element-form.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="111">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-03T13:43:08+00:00</t>
+    <t>2024-06-04T08:55:54+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R5/extensibility.html) for a list).</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>http://ltsi.univ-rennes.fr/ValueSet/forme-pharmaceutique-valueset</t>
   </si>
   <si>
     <t xml:space="preserve">ext-1
@@ -695,7 +701,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="21.57421875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="19.625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="61.8671875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
@@ -1312,13 +1318,11 @@
         <v>75</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="Y6" t="s" s="2">
-        <v>75</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="Y6" s="2"/>
       <c r="Z6" t="s" s="2">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="AA6" t="s" s="2">
         <v>75</v>
@@ -1345,13 +1349,13 @@
         <v>82</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AL6" t="s" s="2">
         <v>101</v>

</xml_diff>

<commit_message>
mis en commentaire de ce CS e91eb803dc5492a6c108f27efa232bf91d6bbecc
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/StructureDefinition-oncofair-element-form.xlsx
+++ b/update-mapping-pn13/ig/StructureDefinition-oncofair-element-form.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="109">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-10T15:21:14+00:00</t>
+    <t>2024-06-11T13:09:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -340,12 +340,6 @@
   </si>
   <si>
     <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R5/extensibility.html) for a list).</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>http://ltsi.univ-rennes.fr/ValueSet/forme-pharmaceutique-valueset</t>
   </si>
   <si>
     <t xml:space="preserve">ext-1
@@ -701,7 +695,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="21.57421875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="61.8671875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="19.625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
@@ -1318,11 +1312,13 @@
         <v>75</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="Y6" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="Y6" t="s" s="2">
+        <v>75</v>
+      </c>
       <c r="Z6" t="s" s="2">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="AA6" t="s" s="2">
         <v>75</v>
@@ -1349,13 +1345,13 @@
         <v>82</v>
       </c>
       <c r="AI6" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AJ6" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="AK6" t="s" s="2">
         <v>108</v>
-      </c>
-      <c r="AJ6" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="AK6" t="s" s="2">
-        <v>110</v>
       </c>
       <c r="AL6" t="s" s="2">
         <v>101</v>

</xml_diff>